<commit_message>
atualizao do ambiente do GKO
</commit_message>
<xml_diff>
--- a/AOL BR Satellites_DM Strategy_Overall_Nutrade.xlsx
+++ b/AOL BR Satellites_DM Strategy_Overall_Nutrade.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T966104\Documents\repos\docs\syngenta-appmap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\syngenta-appmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Transaction Data'!$A$2:$D$141</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -740,7 +740,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1340">
+  <dxfs count="1319">
     <dxf>
       <fill>
         <patternFill>
@@ -771,6 +771,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -805,6 +812,33 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -839,6 +873,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -860,231 +908,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12336,10 +12159,10 @@
   <dimension ref="A1:G310"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B179" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C212" sqref="C212"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -16825,7 +16648,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4 A15 A5:D5 A10:A11 A16:D22 D10:D11 A6:B9 D6:D8">
+  <conditionalFormatting sqref="A15 A4 A5:D5 A10:A11 A16:D22 D10:D11 A6:B9 D6:D8">
     <cfRule type="colorScale" priority="2158">
       <colorScale>
         <cfvo type="min"/>
@@ -29961,10 +29784,10 @@
   <dimension ref="A1:G395"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B330" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C385" sqref="C385"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -42368,12 +42191,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006E566B1B11003D458521C689EEF57D67" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d2c0f041f8bc1087a2191dd4f24c8cca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -42422,6 +42239,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FADFE7A-42F0-49CE-85AD-FE8539B2D273}">
   <ds:schemaRefs>
@@ -42431,20 +42254,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EB06F46-2324-4F19-BEF0-F8AF4A892011}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4AF0366-0C55-4FAD-9098-DED1E75E3D14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42457,4 +42266,18 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EB06F46-2324-4F19-BEF0-F8AF4A892011}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>